<commit_message>
implement in lazy mode permission
</commit_message>
<xml_diff>
--- a/dev/tools/legacy_permissions/data/usecases.xlsx
+++ b/dev/tools/legacy_permissions/data/usecases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19700" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="usecases" sheetId="1" r:id="rId1"/>
@@ -2179,7 +2179,18 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2456,7 +2467,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>